<commit_message>
statistiche aggiornate con 12 casi
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schia\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A6406D-1E12-43D1-A963-7142BF765609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BBE1BF-F108-4633-BB8B-FE78161E69B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="48">
   <si>
     <t>Fidelity</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>1.23</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>3.43</t>
+  </si>
+  <si>
+    <t>2.34</t>
+  </si>
+  <si>
+    <t>1.8</t>
   </si>
 </sst>
 </file>
@@ -488,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="M78" sqref="M78"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="M88" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,6 +1210,9 @@
       <c r="G68">
         <v>3</v>
       </c>
+      <c r="J68" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B70">
@@ -1218,6 +1233,9 @@
       <c r="G70">
         <v>5</v>
       </c>
+      <c r="J70" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B72">
@@ -1237,6 +1255,9 @@
       </c>
       <c r="G72">
         <v>7</v>
+      </c>
+      <c r="J72" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -1261,6 +1282,9 @@
       <c r="G75">
         <v>3</v>
       </c>
+      <c r="J75" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
@@ -1281,6 +1305,9 @@
       <c r="G77">
         <v>5</v>
       </c>
+      <c r="J77" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
@@ -1301,8 +1328,11 @@
       <c r="G79">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J79" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>39</v>
       </c>
@@ -1324,8 +1354,11 @@
       <c r="G82">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>6</v>
       </c>
@@ -1344,8 +1377,11 @@
       <c r="G84">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>6</v>
       </c>
@@ -1363,6 +1399,9 @@
       </c>
       <c r="G86">
         <v>7</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>